<commit_message>
Audit Tied to Rentrak
Making new deliverable template that links to Rentrak
</commit_message>
<xml_diff>
--- a/tables/MSOs.xlsx
+++ b/tables/MSOs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>AT&amp;T</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +151,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,6 +199,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -246,7 +257,9 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C37" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C37"/>
+  <sortState ref="A2:C37">
+    <sortCondition ref="C1:C37"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" name="mso"/>
     <tableColumn id="2" name="mso_no"/>
@@ -546,8 +559,8 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,52 +587,55 @@
       <c r="B2">
         <v>144</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="G2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>135</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>68</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>108</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>58</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3"/>
       <c r="G7" t="s">
@@ -628,24 +644,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>109</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="G8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>49</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
         <v>39</v>
@@ -653,13 +667,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="G10" t="s">
         <v>39</v>
@@ -667,33 +678,30 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>162</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>58</v>
+      </c>
       <c r="G11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>150</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>39</v>
@@ -701,48 +709,46 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>120</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="G14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>141</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>111</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>165</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="G18" t="s">
         <v>39</v>
@@ -750,133 +756,130 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>131</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>160</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>119</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>47</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>143</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
-        <v>182</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>117</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>182</v>
+      </c>
       <c r="G29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>62</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31">
-        <v>176</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>62</v>
+      </c>
       <c r="G31" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>114</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>60</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="G33" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
We are stable right now
Corrected issue where the pd.duplicated was fucking up for Charter.
Should be good accross board. Need to double check.
</commit_message>
<xml_diff>
--- a/tables/MSOs.xlsx
+++ b/tables/MSOs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>AT&amp;T</t>
   </si>
@@ -140,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,14 +151,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -190,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,9 +191,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -560,7 +549,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +576,9 @@
       <c r="B2">
         <v>144</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="G2" t="s">
         <v>39</v>
       </c>
@@ -610,7 +601,9 @@
       <c r="B4">
         <v>50</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -619,7 +612,9 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -628,7 +623,9 @@
       <c r="B6">
         <v>120</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -637,7 +634,9 @@
       <c r="B7">
         <v>60</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" t="s">
         <v>39</v>
       </c>

</xml_diff>